<commit_message>
Update sample data and description
</commit_message>
<xml_diff>
--- a/sampleData/Population Pyramid Sample Data with Ref.xlsx
+++ b/sampleData/Population Pyramid Sample Data with Ref.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F3BF5B-E2EC-4CA1-A322-15DCDD65000A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1851" windowWidth="27429" windowHeight="11751" xr2:uid="{DB55F583-BD66-42A0-85A9-96061EF13B75}"/>
+    <workbookView xWindow="-25515" yWindow="1500" windowWidth="25545" windowHeight="14445" xr2:uid="{DB55F583-BD66-42A0-85A9-96061EF13B75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="spread">Sheet1!$D$21</definedName>
+    <definedName name="spread">Sheet1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="24">
   <si>
     <t>Age</t>
   </si>
@@ -87,10 +88,13 @@
     <t>A85+</t>
   </si>
   <si>
-    <t>FemaleRef</t>
-  </si>
-  <si>
-    <t>MaleRef</t>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Reference</t>
   </si>
 </sst>
 </file>
@@ -101,7 +105,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,52 +120,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor theme="0" tint="-0.14999847407452621"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -170,147 +142,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="2">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -326,16 +171,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93F70379-0EEB-4940-9B1C-402199547765}" name="Table1" displayName="Table1" ref="A1:E19" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E19" xr:uid="{36245C07-4A24-48FF-B295-AFF0EF86F68E}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0223CC44-7BEB-47A1-B866-4DC31D0A143C}" name="Age" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{21DAB12A-446E-41D5-ABE0-EB5591F827C7}" name="Female" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{EC397243-6DFA-4173-AC9A-631C99C21ACE}" name="Male" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{C15998EB-9A0E-4BDD-AFC4-089713DE6D74}" name="FemaleRef" dataDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{22D2C5AE-77F8-4352-BC97-CD95E6680033}" name="MaleRef" dataDxfId="0" dataCellStyle="Comma"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7BE5325-C609-49E6-A3CE-135124FBFFAB}" name="Table1" displayName="Table1" ref="A1:D37" totalsRowShown="0">
+  <autoFilter ref="A1:D37" xr:uid="{D7BE5325-C609-49E6-A3CE-135124FBFFAB}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{BE44DE7D-C9A3-4664-9B13-D9562FA4238E}" name="Age"/>
+    <tableColumn id="2" xr3:uid="{E148ED07-FA8D-4756-A098-8C4D663C88B9}" name="Gender"/>
+    <tableColumn id="3" xr3:uid="{C91C5E97-D4DB-4C1E-84E1-48372A3F0A0E}" name="Value" dataDxfId="0" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{9AEE30FD-F368-4AD8-8B4A-1FED45F40944}" name="Reference" dataDxfId="1" dataCellStyle="Comma"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -636,344 +480,536 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC3DF753-1915-444E-B656-727BF4F964DD}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.3046875" customWidth="1"/>
-    <col min="5" max="5" width="9.4609375" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
         <v>6085.9999999999991</v>
-      </c>
-      <c r="C2" s="6">
-        <v>6592</v>
       </c>
       <c r="D2" s="1">
         <v>5092.6310213741963</v>
       </c>
-      <c r="E2" s="1">
-        <v>4133.9968306058936</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
         <v>5233</v>
-      </c>
-      <c r="C3" s="3">
-        <v>5558</v>
       </c>
       <c r="D3" s="1">
         <v>4441.7313986879517</v>
       </c>
-      <c r="E3" s="1">
-        <v>6991.1531996550129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
         <v>4956</v>
-      </c>
-      <c r="C4" s="2">
-        <v>4902</v>
       </c>
       <c r="D4" s="1">
         <v>5228.3391673624928</v>
       </c>
-      <c r="E4" s="1">
-        <v>4109.217632841126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
         <v>6053</v>
-      </c>
-      <c r="C5" s="3">
-        <v>5947</v>
       </c>
       <c r="D5" s="1">
         <v>5581.6500249331857</v>
       </c>
-      <c r="E5" s="1">
-        <v>4582.0012167992627</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
         <v>12142</v>
-      </c>
-      <c r="C6" s="2">
-        <v>10182</v>
       </c>
       <c r="D6" s="1">
         <v>10651.709613424086</v>
       </c>
-      <c r="E6" s="1">
-        <v>10036.059331509025</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" s="3" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
         <v>14395</v>
-      </c>
-      <c r="C7" s="3">
-        <v>13777</v>
       </c>
       <c r="D7" s="1">
         <v>19985.633064262118</v>
       </c>
-      <c r="E7" s="1">
-        <v>14788.103081971973</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
         <v>12377</v>
-      </c>
-      <c r="C8" s="2">
-        <v>13134</v>
       </c>
       <c r="D8" s="1">
         <v>8505.6646411218935</v>
       </c>
-      <c r="E8" s="1">
-        <v>10508.695108535583</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" s="3" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
         <v>9564</v>
-      </c>
-      <c r="C9" s="3">
-        <v>9726</v>
       </c>
       <c r="D9" s="1">
         <v>7513.3848247621236</v>
       </c>
-      <c r="E9" s="1">
-        <v>11323.435095689878</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" s="2" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2">
-        <v>8172</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
         <v>8172</v>
       </c>
       <c r="D10" s="1">
         <v>10319.100892181619</v>
       </c>
-      <c r="E10" s="1">
-        <v>9937.5782492957132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" s="3" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
         <v>7092</v>
-      </c>
-      <c r="C11" s="3">
-        <v>7260</v>
       </c>
       <c r="D11" s="1">
         <v>5610.9796174276153</v>
       </c>
-      <c r="E11" s="1">
-        <v>4457.4532301483296</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
         <v>6135</v>
-      </c>
-      <c r="C12" s="2">
-        <v>6327</v>
       </c>
       <c r="D12" s="1">
         <v>6201.2102254777046</v>
       </c>
-      <c r="E12" s="1">
-        <v>7250.4586298977274</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" s="3" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
         <v>4834</v>
-      </c>
-      <c r="C13" s="3">
-        <v>5094</v>
       </c>
       <c r="D13" s="1">
         <v>5904.6872412354423</v>
       </c>
-      <c r="E13" s="1">
-        <v>4815.9385822771828</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
         <v>4315</v>
-      </c>
-      <c r="C14" s="2">
-        <v>4047</v>
       </c>
       <c r="D14" s="1">
         <v>4405.8456303047433</v>
       </c>
-      <c r="E14" s="1">
-        <v>4656.5661245530218</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A15" s="3" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
         <v>4260</v>
-      </c>
-      <c r="C15" s="3">
-        <v>3693</v>
       </c>
       <c r="D15" s="1">
         <v>3783.3279218754033</v>
       </c>
-      <c r="E15" s="1">
-        <v>2531.685740126587</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
         <v>3286</v>
-      </c>
-      <c r="C16" s="2">
-        <v>2783</v>
       </c>
       <c r="D16" s="1">
         <v>4404.5466749523166</v>
       </c>
-      <c r="E16" s="1">
-        <v>3268.8835496400179</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A17" s="3" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
         <v>2601</v>
-      </c>
-      <c r="C17" s="3">
-        <v>2089</v>
       </c>
       <c r="D17" s="1">
         <v>3508.5109993041829</v>
       </c>
-      <c r="E17" s="1">
-        <v>2186.9826315069904</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A18" s="2" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
         <v>1936</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1518</v>
       </c>
       <c r="D18" s="1">
         <v>2649.4809022509844</v>
       </c>
-      <c r="E18" s="1">
-        <v>1773.1346391530906</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A19" s="4" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
         <v>2155</v>
-      </c>
-      <c r="C19" s="4">
-        <v>1312</v>
       </c>
       <c r="D19" s="1">
         <v>1565.5235685062135</v>
       </c>
-      <c r="E19" s="1">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>6592</v>
+      </c>
+      <c r="D20" s="1">
+        <v>4133.9968306058936</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5558</v>
+      </c>
+      <c r="D21" s="1">
+        <v>6991.1531996550129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4902</v>
+      </c>
+      <c r="D22" s="1">
+        <v>4109.217632841126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1">
+        <v>5947</v>
+      </c>
+      <c r="D23" s="1">
+        <v>4582.0012167992627</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>10182</v>
+      </c>
+      <c r="D24" s="1">
+        <v>10036.059331509025</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1">
+        <v>13777</v>
+      </c>
+      <c r="D25" s="1">
+        <v>14788.103081971973</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1">
+        <v>13134</v>
+      </c>
+      <c r="D26" s="1">
+        <v>10508.695108535583</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1">
+        <v>9726</v>
+      </c>
+      <c r="D27" s="1">
+        <v>11323.435095689878</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1">
+        <v>8172</v>
+      </c>
+      <c r="D28" s="1">
+        <v>9937.5782492957132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1">
+        <v>7260</v>
+      </c>
+      <c r="D29" s="1">
+        <v>4457.4532301483296</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="1">
+        <v>6327</v>
+      </c>
+      <c r="D30" s="1">
+        <v>7250.4586298977274</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1">
+        <v>5094</v>
+      </c>
+      <c r="D31" s="1">
+        <v>4815.9385822771828</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1">
+        <v>4047</v>
+      </c>
+      <c r="D32" s="1">
+        <v>4656.5661245530218</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1">
+        <v>3693</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2531.685740126587</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2783</v>
+      </c>
+      <c r="D34" s="1">
+        <v>3268.8835496400179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2089</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2186.9826315069904</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1518</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1773.1346391530906</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1312</v>
+      </c>
+      <c r="D37" s="1">
         <v>1062.7225851095384</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>